<commit_message>
[filter] - [`not contain`](../flowcontrols/filter.#description): handle text delimiter being used as control. - [`contain`](../flowcontrols/filter.#description): handle text delimiter being used as control.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-script.xlsx
+++ b/template/nexial-script.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64102" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65755" uniqueCount="548">
   <si>
     <t>description</t>
   </si>
@@ -1718,7 +1718,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1867" x14ac:knownFonts="1">
+  <fonts count="1915" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -13511,8 +13511,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="3175">
+  <fills count="3256">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -31500,8 +31803,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3663">
+  <borders count="3759">
     <border>
       <left/>
       <right/>
@@ -35027,6 +35789,984 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -68790,7 +70530,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1893">
+  <cellXfs count="1941">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -74439,52 +76179,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="3147" fontId="1850" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1851" fillId="3150" borderId="3638" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1852" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3638" fillId="3150" fontId="1851" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1852" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1853" fillId="3153" borderId="3642" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3642" fillId="3153" fontId="1853" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1854" fillId="3156" borderId="3646" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3646" fillId="3156" fontId="1854" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1855" fillId="3159" borderId="3650" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3650" fillId="3159" fontId="1855" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1856" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1856" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1857" fillId="3162" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3162" fontId="1857" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1858" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1859" fillId="3165" borderId="3654" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1860" fillId="3156" borderId="3658" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1861" fillId="3168" borderId="3662" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1862" fillId="3168" borderId="3662" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1863" fillId="3159" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1864" fillId="3171" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1865" fillId="3159" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1866" fillId="3174" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1858" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3654" fillId="3165" fontId="1859" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3658" fillId="3156" fontId="1860" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3662" fillId="3168" fontId="1861" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3662" fillId="3168" fontId="1862" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3159" fontId="1863" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3171" fontId="1864" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3159" fontId="1865" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3174" fontId="1866" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3670" fillId="3177" fontId="1867" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1868" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3674" fillId="3180" fontId="1869" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3678" fillId="3183" fontId="1870" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3682" fillId="3186" fontId="1871" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1872" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3189" fontId="1873" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1874" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3686" fillId="3192" fontId="1875" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3690" fillId="3183" fontId="1876" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3694" fillId="3195" fontId="1877" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3694" fillId="3195" fontId="1878" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3186" fontId="1879" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3198" fontId="1880" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3186" fontId="1881" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3201" fontId="1882" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3702" fillId="3204" fontId="1883" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1884" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3706" fillId="3207" fontId="1885" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3710" fillId="3210" fontId="1886" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3714" fillId="3213" fontId="1887" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1888" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3216" fontId="1889" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1890" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3718" fillId="3219" fontId="1891" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3722" fillId="3210" fontId="1892" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3726" fillId="3222" fontId="1893" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3726" fillId="3222" fontId="1894" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3213" fontId="1895" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3225" fontId="1896" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3213" fontId="1897" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="3228" fontId="1898" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1899" fillId="3231" borderId="3734" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1900" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1901" fillId="3234" borderId="3738" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1902" fillId="3237" borderId="3742" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1903" fillId="3240" borderId="3746" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1904" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1905" fillId="3243" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1906" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1907" fillId="3246" borderId="3750" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1908" fillId="3237" borderId="3754" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1909" fillId="3249" borderId="3758" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1910" fillId="3249" borderId="3758" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1911" fillId="3240" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1912" fillId="3252" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1913" fillId="3240" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1914" fillId="3255" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>